<commit_message>
Mise à jour de l'audit
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastien/Documents (local)/OpenClassRooms/Projets et Certificats/Projet 4/Projet 4 - La Chouette Agence/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastien/Documents (local)/OpenClassRooms/Projets et Certificats/Projet 4/Projet 4 - La Chouette Agence/Starting website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813DB655-F5EC-3A46-B8AE-593EF9E0A080}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792F6CFD-0F3E-134F-9107-7F6C72209AEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="500" windowWidth="27860" windowHeight="16540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23360" windowHeight="27320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="100">
   <si>
     <t>Catégorie</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t>Accessibilité</t>
-  </si>
-  <si>
-    <t>Footer - Contraste</t>
   </si>
   <si>
     <t>Pas de Titre dans le &lt;head&gt;</t>
@@ -194,9 +191,6 @@
     <t>utiliser une police d'écriture plus grande.</t>
   </si>
   <si>
-    <t>les polices inférieures à 12 px forcent les utilisateurs mobiles à zoomer pour lire. Ayez + de 60% de votre page avec une police supérieure à 12px.</t>
-  </si>
-  <si>
     <t>https://github.com/GoogleChrome/lighthouse/blob/master/lighthouse-core/audits/seo/font-size.js</t>
   </si>
   <si>
@@ -206,9 +200,6 @@
     <t>Taille des liens trop petite pour cliquer en tactile</t>
   </si>
   <si>
-    <t>les zones de clic doivent faire à minim 48px X 48pox et avoir de l'espace autours afin de permettre le clic mobile.</t>
-  </si>
-  <si>
     <t>insérer un padding et augmenter la taille de surface clicable.</t>
   </si>
   <si>
@@ -245,9 +236,6 @@
     <t>Absence de balise "defer" ou "async" pour les gestion des &lt;script&gt; en chargement</t>
   </si>
   <si>
-    <t>indiquer si le &lt;script&gt; doit se charger à l'ouverture de la page ou si ce dernier peut-être différé.</t>
-  </si>
-  <si>
     <t>ajouter "defer" ou "async" dans vos &lt;script&gt; html</t>
   </si>
   <si>
@@ -272,9 +260,6 @@
     <t>Utilisation abusive de z-index</t>
   </si>
   <si>
-    <t>l’ordre des z-index et la position hors-écran NE DOIVENT PAS être utilisées aux seules fins de visibilité</t>
-  </si>
-  <si>
     <t>Utiliser les attributs &lt;hidden&gt; ou les propriétés de style &lt;visibility&gt; ou &lt;display&gt;.</t>
   </si>
   <si>
@@ -308,7 +293,85 @@
     <t>Vérifier l'intégration de vos images avec votre page</t>
   </si>
   <si>
-    <t>Redimensionner le logi afin de ne plus avoir de faux bords</t>
+    <t>Head - keywords</t>
+  </si>
+  <si>
+    <t>dupplication de mots clés</t>
+  </si>
+  <si>
+    <t>épurés cette ablise meta avec des mots clés ciblés</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578338-reconnaissez-les-differents-types-de-mots-cles</t>
+  </si>
+  <si>
+    <t>Ciblés les mots clés</t>
+  </si>
+  <si>
+    <t>L’ordre des z-index et la position hors-écran NE DOIVENT PAS être utilisées aux seules fins de visibilité</t>
+  </si>
+  <si>
+    <t>Indiquer si le &lt;script&gt; doit se charger à l'ouverture de la page ou si ce dernier peut-être différé.</t>
+  </si>
+  <si>
+    <t>Les polices inférieures à 12 px forcent les utilisateurs mobiles à zoomer pour lire. Ayez + de 60% de votre page avec une police supérieure à 12px.</t>
+  </si>
+  <si>
+    <t>Les zones de clic doivent faire à minim 48px X 48pox et avoir de l'espace autours afin de permettre le clic mobile.</t>
+  </si>
+  <si>
+    <t>Réduire la taille des fichiers HTML, CSS, JS…</t>
+  </si>
+  <si>
+    <t>Utiliser un outil de réduction de votre code.</t>
+  </si>
+  <si>
+    <t>Utiliser un outil gratuit en ligne pour minimiser votre code et amélioer le chargement.</t>
+  </si>
+  <si>
+    <t>Redimensionner le logo afin de ne plus avoir de faux bords</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5922626-optimisez-le-referencement-de-votre-site-seo-en-ameliorant-ses-performances-techniques/6055231-allegez-les-pages-de-votre-site</t>
+  </si>
+  <si>
+    <t>Head - Analytics</t>
+  </si>
+  <si>
+    <t>Absence d'outls de suivi SEO.</t>
+  </si>
+  <si>
+    <t>Utiliser des outils type Google Anlaytics afin de suivre les performances de votre site.</t>
+  </si>
+  <si>
+    <t>Ajouter un extrait de code type Google Analytics afin de suivre vos performances régulièrement.</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5604431-installez-les-bons-outils</t>
+  </si>
+  <si>
+    <t>Footer - Contraste + Page Contact</t>
+  </si>
+  <si>
+    <t>Footer trop chargé donc utilisation du budget crawling inutile.</t>
+  </si>
+  <si>
+    <t>Éviter les annuaires sur vos pages afin de ne pas gaspiller votre budget crawling.</t>
+  </si>
+  <si>
+    <t>Réduire vos liens à des liens de qualités uniquement.</t>
+  </si>
+  <si>
+    <t>https://openclassrooms.com/fr/courses/5561431-augmentez-votre-trafic-grace-au-referencement-naturel-seo/5578346-augmentez-lautorite-de-votre-site</t>
+  </si>
+  <si>
+    <t>Utilisation abusives de commentaires</t>
+  </si>
+  <si>
+    <t>un code bien rédiger n'a pas besoin de commentaire.</t>
+  </si>
+  <si>
+    <t>Retirer vos commentaires et reprenez la structure de votre code (bis accessibilité)</t>
   </si>
 </sst>
 </file>
@@ -394,7 +457,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,26 +482,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -655,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z987"/>
+  <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -669,8 +731,8 @@
     <col min="4" max="4" width="114.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="71" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="112.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="26" width="10.5703125" style="15" customWidth="1"/>
-    <col min="27" max="16384" width="11.28515625" style="15"/>
+    <col min="7" max="26" width="10.5703125" style="3" customWidth="1"/>
+    <col min="27" max="16384" width="11.28515625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
@@ -692,345 +754,437 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="E2" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>22</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="8" t="s">
+      <c r="B3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>12</v>
+      <c r="F3" s="9" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>15</v>
+      <c r="B4" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>12</v>
+        <v>77</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>28</v>
+      <c r="B6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>68</v>
+      <c r="B7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15" customHeight="1">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="8"/>
+      <c r="B8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="B9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="8"/>
+      <c r="B10" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:26" ht="15" customHeight="1">
+      <c r="A12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="F12" s="11" t="s">
         <v>35</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A12" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="7" t="s">
+      <c r="B13" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>49</v>
+      <c r="F13" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="B14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>51</v>
       </c>
+      <c r="D14" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="E14" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>53</v>
+        <v>45</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1">
+      <c r="A17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>64</v>
+      <c r="D17" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1">
-      <c r="A16" s="2" t="s">
+    <row r="18" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>41</v>
       </c>
+      <c r="D18" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>43</v>
+      </c>
     </row>
-    <row r="17" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A17" s="2" t="s">
+    <row r="19" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A19" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>46</v>
+      <c r="B19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="19" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="20" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="21" spans="1:6" ht="15.75" customHeight="1"/>
-    <row r="22" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="20" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A20" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A21" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A22" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
@@ -1996,19 +2150,22 @@
     <row r="985" ht="15.75" customHeight="1"/>
     <row r="986" ht="15.75" customHeight="1"/>
     <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{991C24E8-E904-CB49-AF3E-A573AE651E30}"/>
-    <hyperlink ref="F6" r:id="rId2" xr:uid="{4723375C-B487-D340-A60A-0079F107FFCB}"/>
-    <hyperlink ref="F11" r:id="rId3" location="1" xr:uid="{8857E384-49BC-4449-B01A-C1D993E6CF81}"/>
-    <hyperlink ref="F16" r:id="rId4" xr:uid="{0D4FD6C5-AB68-564E-B524-1D839CDEC8D7}"/>
-    <hyperlink ref="F17" r:id="rId5" xr:uid="{B2240EBB-228D-ED44-B02E-622E190311E3}"/>
-    <hyperlink ref="F13" r:id="rId6" xr:uid="{C91D65D6-6CE9-5E4E-945A-F1CB1C42FAC4}"/>
-    <hyperlink ref="F14" r:id="rId7" xr:uid="{CB4103B3-9E04-1545-8E97-FD9DF25FEB6A}"/>
-    <hyperlink ref="F12" r:id="rId8" xr:uid="{C48E88E2-6481-4640-8550-7A761701BCB2}"/>
-    <hyperlink ref="G12" r:id="rId9" xr:uid="{0DF24874-A22B-5D49-A1F9-EFF6B9148A4C}"/>
-    <hyperlink ref="F15" r:id="rId10" xr:uid="{31AFCD03-751A-DB4E-96B6-923C96A176A4}"/>
-    <hyperlink ref="F7" r:id="rId11" xr:uid="{F0E0C6FC-F165-0844-938F-BC62AFB357B4}"/>
+    <hyperlink ref="F7" r:id="rId2" xr:uid="{4723375C-B487-D340-A60A-0079F107FFCB}"/>
+    <hyperlink ref="F12" r:id="rId3" location="1" xr:uid="{8857E384-49BC-4449-B01A-C1D993E6CF81}"/>
+    <hyperlink ref="F17" r:id="rId4" xr:uid="{0D4FD6C5-AB68-564E-B524-1D839CDEC8D7}"/>
+    <hyperlink ref="F18" r:id="rId5" xr:uid="{B2240EBB-228D-ED44-B02E-622E190311E3}"/>
+    <hyperlink ref="F14" r:id="rId6" xr:uid="{C91D65D6-6CE9-5E4E-945A-F1CB1C42FAC4}"/>
+    <hyperlink ref="F15" r:id="rId7" xr:uid="{CB4103B3-9E04-1545-8E97-FD9DF25FEB6A}"/>
+    <hyperlink ref="F13" r:id="rId8" xr:uid="{C48E88E2-6481-4640-8550-7A761701BCB2}"/>
+    <hyperlink ref="G13" r:id="rId9" xr:uid="{0DF24874-A22B-5D49-A1F9-EFF6B9148A4C}"/>
+    <hyperlink ref="F16" r:id="rId10" xr:uid="{31AFCD03-751A-DB4E-96B6-923C96A176A4}"/>
+    <hyperlink ref="F8" r:id="rId11" xr:uid="{F0E0C6FC-F165-0844-938F-BC62AFB357B4}"/>
+    <hyperlink ref="F4" r:id="rId12" xr:uid="{A0B90625-CE51-7D4E-99EC-F99C60AA801B}"/>
+    <hyperlink ref="F19" r:id="rId13" xr:uid="{BC74307F-224A-8443-A22B-4D2798D42DE5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Nettoygae JS et script pour optimisation
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastien/Documents (local)/OpenClassRooms/Projets et Certificats/Projet 4/Projet 4 - La Chouette Agence/Starting website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792F6CFD-0F3E-134F-9107-7F6C72209AEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2648A976-9EE7-A94C-816C-29673020E5C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="23360" windowHeight="27320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
   <si>
     <t>Catégorie</t>
   </si>
@@ -372,6 +372,15 @@
   </si>
   <si>
     <t>Retirer vos commentaires et reprenez la structure de votre code (bis accessibilité)</t>
+  </si>
+  <si>
+    <t>Libraries Jquery obsolètes failles présentes.</t>
+  </si>
+  <si>
+    <t>garder les librarires à jour afin d'éviter les vulnérabilités.</t>
+  </si>
+  <si>
+    <t>Mettre à jour les libraires Jquery</t>
   </si>
 </sst>
 </file>
@@ -720,7 +729,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1185,7 +1194,23 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="23" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A23" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>102</v>
+      </c>
+    </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="26" spans="1:6" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Mise à jour Audit SEO
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastien/Documents (local)/OpenClassRooms/Projets et Certificats/Projet 4/Projet 4 - La Chouette Agence/Starting website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2648A976-9EE7-A94C-816C-29673020E5C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6669E4-B1D2-3E46-BFB6-12F348CE52B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23360" windowHeight="27320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="42240" windowHeight="27320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -152,9 +152,6 @@
     <t>Donner un nom unique à vos liens afin qu'ils se différencient lors de la lecture par l'assistant.</t>
   </si>
   <si>
-    <t>Remplacer le nom de vos fichiers html par un nom unique.</t>
-  </si>
-  <si>
     <t>https://dequeuniversity.com/rules/axe/3.3/link-name</t>
   </si>
   <si>
@@ -381,6 +378,9 @@
   </si>
   <si>
     <t>Mettre à jour les libraires Jquery</t>
+  </si>
+  <si>
+    <t>Remplacer le nom de vos fichiers html par un nom unique (icone réseaux sociaux)</t>
   </si>
 </sst>
 </file>
@@ -729,7 +729,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -789,7 +789,7 @@
         <v>7</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>19</v>
@@ -809,7 +809,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>8</v>
@@ -829,19 +829,19 @@
         <v>7</v>
       </c>
       <c r="B4" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="D4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="E4" s="10" t="s">
+      <c r="F4" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
@@ -849,7 +849,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>14</v>
@@ -869,7 +869,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>13</v>
@@ -898,10 +898,10 @@
         <v>25</v>
       </c>
       <c r="E7" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
@@ -909,19 +909,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="E8" s="6" t="s">
+      <c r="F8" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
@@ -929,16 +929,16 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="E9" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="F9" s="3"/>
     </row>
@@ -947,10 +947,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -961,16 +961,16 @@
         <v>7</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="D11" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F11" s="3"/>
     </row>
@@ -979,19 +979,19 @@
         <v>6</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="D12" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="F12" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
@@ -999,22 +999,22 @@
         <v>6</v>
       </c>
       <c r="B13" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="D13" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="10" t="s">
+      <c r="F13" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="11" t="s">
+      <c r="G13" s="4" t="s">
         <v>55</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
@@ -1022,19 +1022,19 @@
         <v>6</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
@@ -1042,19 +1042,19 @@
         <v>6</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="E15" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="F15" s="11" t="s">
         <v>49</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
@@ -1062,19 +1062,19 @@
         <v>6</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="F16" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1">
@@ -1082,19 +1082,19 @@
         <v>6</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="D17" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1">
@@ -1102,19 +1102,19 @@
         <v>6</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="6" t="s">
+      <c r="F18" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1">
@@ -1122,19 +1122,19 @@
         <v>6</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="E19" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>84</v>
-      </c>
       <c r="F19" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1">
@@ -1142,19 +1142,19 @@
         <v>6</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="D20" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="E20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="F20" s="12" t="s">
         <v>90</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1">
@@ -1162,19 +1162,19 @@
         <v>6</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="E21" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="F21" s="12" t="s">
         <v>95</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1">
@@ -1182,16 +1182,16 @@
         <v>6</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="E22" s="15" t="s">
         <v>98</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1">
@@ -1199,16 +1199,16 @@
         <v>6</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="E23" s="7" t="s">
         <v>101</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Transfert du script en bas de page
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastien/Documents (local)/OpenClassRooms/Projets et Certificats/Projet 4/Projet 4 - La Chouette Agence/Starting website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC6669E4-B1D2-3E46-BFB6-12F348CE52B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AFD5A6-1480-4E44-8AF6-E25DB6DEA702}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="42240" windowHeight="27320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -729,7 +729,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A10" sqref="A6:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -865,114 +865,114 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="12" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="11" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="3"/>
+      <c r="F9" s="12"/>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="3"/>
+      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1">
       <c r="A12" s="13" t="s">
@@ -1058,22 +1058,22 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="11" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1118,22 +1118,22 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="11" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correction structure h1 h2 et h3
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebastien/Documents (local)/OpenClassRooms/Projets et Certificats/Projet 4/Projet 4 - La Chouette Agence/Starting website/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81AFD5A6-1480-4E44-8AF6-E25DB6DEA702}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B070FA3C-28DE-614A-BF38-4320AA96E78E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="42240" windowHeight="27320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="105">
   <si>
     <t>Catégorie</t>
   </si>
@@ -381,6 +381,12 @@
   </si>
   <si>
     <t>Remplacer le nom de vos fichiers html par un nom unique (icone réseaux sociaux)</t>
+  </si>
+  <si>
+    <t>Librairies BootStrap Obsolètes</t>
+  </si>
+  <si>
+    <t>garder votre code à jour</t>
   </si>
 </sst>
 </file>
@@ -729,7 +735,7 @@
   <dimension ref="A1:Z988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A6:F10"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1211,7 +1217,24 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="15.75" customHeight="1"/>
+    <row r="24" spans="1:6" ht="15.75" customHeight="1">
+      <c r="A24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="26" spans="1:6" ht="15.75" customHeight="1"/>
     <row r="27" spans="1:6" ht="15.75" customHeight="1"/>

</xml_diff>